<commit_message>
done few more qsns
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHIT\Desktop\lovebabbardsaSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E1E180-9D9C-42EF-8A21-7D4EC62A2402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C67355-9A9C-4667-B959-B178B3B48FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3564" yWindow="2772" windowWidth="17280" windowHeight="8964" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="B188" sqref="B188"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2901,7 +2901,7 @@
         <v>98</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="21">
@@ -2912,7 +2912,7 @@
         <v>99</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21">
@@ -2923,7 +2923,7 @@
         <v>100</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="21">
@@ -2934,7 +2934,7 @@
         <v>101</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21">
@@ -2945,7 +2945,7 @@
         <v>102</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="21">
@@ -3789,7 +3789,7 @@
         <v>180</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3800,7 +3800,7 @@
         <v>181</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">
@@ -3811,7 +3811,7 @@
         <v>182</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21">
@@ -3822,7 +3822,7 @@
         <v>183</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21">
@@ -4075,7 +4075,7 @@
         <v>206</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="21">

</xml_diff>